<commit_message>
Changed pandas reader engine to openpyxl
</commit_message>
<xml_diff>
--- a/translator/Book1-translated.xlsx
+++ b/translator/Book1-translated.xlsx
@@ -50,7 +50,6 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -66,6 +65,74 @@
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -386,7 +453,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Anhui Transportation Holding Group Company Limited</t>
+          <t>安徽交通控股集团有限公司</t>
         </is>
       </c>
     </row>
@@ -398,7 +465,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Beijing Future Science Park Development Group Co., Ltd.</t>
+          <t>北京未来科学园发展集团有限公司</t>
         </is>
       </c>
     </row>
@@ -410,7 +477,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Beijing Grain Group Co., Ltd.</t>
+          <t>北京五谷集团有限公司</t>
         </is>
       </c>
     </row>
@@ -422,7 +489,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Beijing State-Owned Assets Management Co., Ltd.</t>
+          <t>北京国有资产管理有限公司</t>
         </is>
       </c>
     </row>
@@ -434,7 +501,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Changchun Urban Development &amp; Investment Holdings (Group) Co., Ltd.</t>
+          <t>长春城市发展投资控股（集团）有限公司</t>
         </is>
       </c>
     </row>
@@ -446,7 +513,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Chengdu Airport Xingcheng Investment Group Co., Ltd.</t>
+          <t>Cheng度airport xing成investment group co., Ltd.</t>
         </is>
       </c>
     </row>
@@ -458,7 +525,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Chengdu Airport Xingcheng Investment Group Co., Ltd.</t>
+          <t>Cheng度airport xing成investment group co., Ltd.</t>
         </is>
       </c>
     </row>
@@ -470,7 +537,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Chengdu Communications Investment Group Corporation Limited</t>
+          <t>成都交通投资集团有限公司</t>
         </is>
       </c>
     </row>
@@ -482,7 +549,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>China Huarong Asset Management Co., Ltd.</t>
+          <t>中国华融资产管理有限公司</t>
         </is>
       </c>
     </row>
@@ -494,7 +561,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Chongqing Nan'an Urban Construction &amp; Development (Group) Co., Ltd.</t>
+          <t>重庆市南岸城市建设发展（集团）有限公司</t>
         </is>
       </c>
     </row>
@@ -506,7 +573,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Dalian Deta Holding Co., Ltd.</t>
+          <t>DA连D ETA holding co., Ltd.</t>
         </is>
       </c>
     </row>
@@ -518,7 +585,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Gansu Provincial Highway Aviation Tourism Investment Group Co., Ltd.</t>
+          <t>甘肃省公路航空旅游投资集团有限公司</t>
         </is>
       </c>
     </row>
@@ -530,7 +597,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Guangdong Hengjian Investment Holding Co., Ltd.</t>
+          <t>GU案G栋he ng见investment holding co., Ltd.</t>
         </is>
       </c>
     </row>
@@ -542,7 +609,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Guangdong Hengjian Investment Holding Co., Ltd.</t>
+          <t>GU案G栋he ng见investment holding co., Ltd.</t>
         </is>
       </c>
     </row>
@@ -554,7 +621,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Guangxi Liuzhou Dongcheng Investment Development Group Co., Ltd.</t>
+          <t>GU案G系L IU周dong成investment development group co., Ltd.</t>
         </is>
       </c>
     </row>
@@ -566,7 +633,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Guangzhou Development District Financial Holdings Group Co., Ltd.</t>
+          <t>广州开发区金融控股集团有限公司</t>
         </is>
       </c>
     </row>
@@ -578,7 +645,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Hanjiang Guotou Group Co., Ltd.</t>
+          <t>H安检GG UO头group co., Ltd.</t>
         </is>
       </c>
     </row>
@@ -590,7 +657,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Hebei Construction &amp; Investment Group Co. Ltd</t>
+          <t>河北建设投资集团有限公司</t>
         </is>
       </c>
     </row>
@@ -602,7 +669,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Hebei Construction &amp; Investment Group Co. Ltd</t>
+          <t>河北建设投资集团有限公司</t>
         </is>
       </c>
     </row>
@@ -614,7 +681,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Hebei State-Owned Assets Holding &amp; Operation Co., Ltd.</t>
+          <t>河北省国有资产控股经营有限公司</t>
         </is>
       </c>
     </row>
@@ -626,7 +693,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Hefei Industry Investment Holding (Group) Co., Ltd.</t>
+          <t>合肥工业投资控股（集团）有限公司</t>
         </is>
       </c>
     </row>
@@ -638,7 +705,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Henan Investment Group Co., Ltd.</t>
+          <t>河南投资集团有限公司</t>
         </is>
       </c>
     </row>
@@ -650,7 +717,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Henan Investment Group Co., Ltd.</t>
+          <t>河南投资集团有限公司</t>
         </is>
       </c>
     </row>
@@ -662,7 +729,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Hengyang City Construction Investment Company Limited</t>
+          <t>衡阳市建设投资有限公司</t>
         </is>
       </c>
     </row>
@@ -674,7 +741,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Huai'an Development Holdings Co.,Ltd</t>
+          <t>淮安发展控股有限公司</t>
         </is>
       </c>
     </row>
@@ -686,7 +753,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Huai'an Traffic Holding Co., Ltd.</t>
+          <t>hu AI按traffic holding co., Ltd.</t>
         </is>
       </c>
     </row>
@@ -698,7 +765,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Jiangsu HanRui Investment Holding Co.,Ltd.</t>
+          <t>江苏汉瑞投资控股有限公司</t>
         </is>
       </c>
     </row>
@@ -710,7 +777,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Jiangsu Jinguan Investment and Development Group Co., Ltd.</t>
+          <t>Jiang苏jin管investment and development group co., Ltd.</t>
         </is>
       </c>
     </row>
@@ -722,7 +789,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Jiangxi Railway Investment Group Corporation</t>
+          <t>江西铁路投资集团公司</t>
         </is>
       </c>
     </row>
@@ -734,7 +801,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Kunming Dianchi Investment Co., Ltd.</t>
+          <t>Kunming Dian吃investment co., Ltd.</t>
         </is>
       </c>
     </row>
@@ -746,7 +813,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Kunming Traffic Investment Co., Ltd.</t>
+          <t>昆明交通投资有限公司</t>
         </is>
       </c>
     </row>
@@ -758,7 +825,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Kunming Traffic Investment Co., Ltd.</t>
+          <t>昆明交通投资有限公司</t>
         </is>
       </c>
     </row>
@@ -770,7 +837,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Kunshan Transportation Development Holding Group Co.,Ltd</t>
+          <t>昆山交通发展控股集团有限公司</t>
         </is>
       </c>
     </row>
@@ -782,7 +849,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Lanzhou Construction Investment (Holding) Group Co., Ltd.</t>
+          <t>兰州建设投资（控股）集团有限公司</t>
         </is>
       </c>
     </row>
@@ -794,7 +861,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Liangshan Development (Holdings) Group Co., Ltd.</t>
+          <t>凉山发展（集团）集团有限公司</t>
         </is>
       </c>
     </row>
@@ -806,7 +873,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Linyi City Construction Investment Group Co., Ltd.</t>
+          <t>临沂市建设投资集团有限公司</t>
         </is>
       </c>
     </row>
@@ -818,7 +885,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Mudanjiang City Investment Group Co., Ltd.</t>
+          <t>牡丹江市投资集团有限公司</t>
         </is>
       </c>
     </row>
@@ -830,7 +897,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Qingdao City Construction Investment (Group) Limited</t>
+          <t>青岛城市建设投资（集团）有限公司</t>
         </is>
       </c>
     </row>
@@ -842,7 +909,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Shanghai Lingang Economic Development (Group) Co., Ltd</t>
+          <t>Shanghai Lin刚economic development (group) co., Ltd</t>
         </is>
       </c>
     </row>
@@ -854,7 +921,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Shanghai Lingang Economic Development (Group) Co., Ltd</t>
+          <t>Shanghai Lin刚economic development (group) co., Ltd</t>
         </is>
       </c>
     </row>
@@ -866,7 +933,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Sichuan Railway Investment Group Co., Ltd.</t>
+          <t>四川铁路投资集团有限公司</t>
         </is>
       </c>
     </row>
@@ -878,7 +945,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Suqian Economic Development Corporation</t>
+          <t>SU纤economic development corporation</t>
         </is>
       </c>
     </row>
@@ -890,7 +957,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Tianjin Binhai New Area Construction and Investment Group Co., Ltd.</t>
+          <t>天津滨海新区建设投资集团有限公司</t>
         </is>
       </c>
     </row>
@@ -902,7 +969,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Weifang Urban Construction and Development Investment Group Co., Ltd.</t>
+          <t>潍坊城市建设发展投资集团有限公司</t>
         </is>
       </c>
     </row>
@@ -914,7 +981,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Wuhan Trading Group Co., Ltd</t>
+          <t>武汉贸易集团有限公司</t>
         </is>
       </c>
     </row>
@@ -926,7 +993,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Wuxi Construction and Development Investment Co., Ltd.</t>
+          <t>无锡市建设发展投资有限公司</t>
         </is>
       </c>
     </row>
@@ -938,7 +1005,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Xuzhou Economic and Technology Development Zone State-Owned Assets Management Co., Ltd.</t>
+          <t>徐州经济技术开发区国有资产管理有限公司</t>
         </is>
       </c>
     </row>
@@ -950,7 +1017,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t xml:space="preserve">Yantai Guofeng Investment </t>
+          <t>Y安泰Guofeng investment</t>
         </is>
       </c>
     </row>
@@ -962,7 +1029,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Yueyang Construction and Investment Group Co., Ltd.</t>
+          <t>岳阳建设投资集团有限公司</t>
         </is>
       </c>
     </row>
@@ -974,7 +1041,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Zhangzhou Transportation Development Group Co., Ltd.</t>
+          <t>漳州交通发展集团有限公司</t>
         </is>
       </c>
     </row>
@@ -986,7 +1053,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Zhongyuan Asset Management Co., Ltd</t>
+          <t>中原资产管理有限公司</t>
         </is>
       </c>
     </row>
@@ -998,7 +1065,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Zhongyuan Yuzi Investment Holding Group Co., Ltd.</t>
+          <t>Z宏远Y U字investment holding group co., Ltd.</t>
         </is>
       </c>
     </row>
@@ -1010,7 +1077,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Zhuhai Huafa Group Co., Ltd.</t>
+          <t>Z胡海hu A法group co., Ltd.</t>
         </is>
       </c>
     </row>
@@ -1022,7 +1089,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Zhuhai Huafa Group Co., Ltd.</t>
+          <t>Z胡海hu A法group co., Ltd.</t>
         </is>
       </c>
     </row>
@@ -1034,7 +1101,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Zhuji State-owned Assets Management Co., Ltd.</t>
+          <t>诸暨市国有资产管理有限公司</t>
         </is>
       </c>
     </row>

</xml_diff>